<commit_message>
Atualização de novos testes após os ajustes das distancias, coordenadas e do algoritmo A*
</commit_message>
<xml_diff>
--- a/Algoritmo_Rota/Planilhas/A_Estrela_Euclidiano/PLN_42_10.xlsx
+++ b/Algoritmo_Rota/Planilhas/A_Estrela_Euclidiano/PLN_42_10.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,30 +429,20 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>inicio</t>
+          <t>Distancia</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Distancia</t>
+          <t>max</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>ativos</t>
+          <t>min</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
-        <is>
-          <t>melhor rota</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>caminho</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
         <is>
           <t>Tempo</t>
         </is>
@@ -463,86 +453,169 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>2422.766666666667</v>
       </c>
       <c r="C2" t="n">
-        <v>3144</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>34, 10, 1, 23, 4, 13, 40, 25, 35, 33</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>12 -&gt; 23 -&gt; 40 -&gt; 35 -&gt; 13 -&gt; 10 -&gt; 4 -&gt; 1 -&gt; 25 -&gt; 33 -&gt; 34 -&gt; 12</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>12 -&gt; 16 -&gt; 17 -&gt; 20 -&gt; 24 -&gt; 23 -&gt; 24 -&gt; 32 -&gt; 41 -&gt; 42 -&gt; 40 -&gt; 39 -&gt; 36 -&gt; 35 -&gt; 29 -&gt; 13 -&gt; 12 -&gt; 11 -&gt; 10 -&gt; 7 -&gt; 4 -&gt; 1 -&gt; 2 -&gt; 3 -&gt; 25 -&gt; 26 -&gt; 33 -&gt; 27 -&gt; 28 -&gt; 34 -&gt; 28 -&gt; 29 -&gt; 13 -&gt; 12</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>0.04143404960632324</v>
+        <v>2679</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2268</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.02985102335611979</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>24</v>
+        <v>2425</v>
       </c>
       <c r="C3" t="n">
-        <v>2345</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>8, 2, 21, 27, 12, 19, 31, 39, 38, 14</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>24 -&gt; 21 -&gt; 14 -&gt; 12 -&gt; 8 -&gt; 2 -&gt; 27 -&gt; 38 -&gt; 39 -&gt; 31 -&gt; 19 -&gt; 24</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>24 -&gt; 23 -&gt; 22 -&gt; 21 -&gt; 18 -&gt; 14 -&gt; 10 -&gt; 11 -&gt; 12 -&gt; 8 -&gt; 5 -&gt; 2 -&gt; 3 -&gt; 25 -&gt; 26 -&gt; 27 -&gt; 28 -&gt; 29 -&gt; 30 -&gt; 37 -&gt; 38 -&gt; 39 -&gt; 38 -&gt; 31 -&gt; 20 -&gt; 19 -&gt; 20 -&gt; 24</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>0.04224061965942383</v>
+        <v>2552</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2364</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0295865535736084</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B4" t="n">
+        <v>2287.866666666667</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2411</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2171</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0326434055964152</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2155.466666666667</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2234</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2080</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.02993044058481852</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2157.3</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2251</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1922</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.03292287190755208</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1786.433333333333</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1949</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1614</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0391965389251709</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>6</v>
       </c>
-      <c r="C4" t="n">
-        <v>2357</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>32, 42, 20, 17, 16, 1, 15, 11, 37, 9</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>6 -&gt; 9 -&gt; 17 -&gt; 16 -&gt; 20 -&gt; 32 -&gt; 42 -&gt; 37 -&gt; 15 -&gt; 11 -&gt; 1 -&gt; 6</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>6 -&gt; 9 -&gt; 13 -&gt; 17 -&gt; 16 -&gt; 17 -&gt; 20 -&gt; 24 -&gt; 32 -&gt; 41 -&gt; 42 -&gt; 40 -&gt; 39 -&gt; 38 -&gt; 37 -&gt; 30 -&gt; 17 -&gt; 16 -&gt; 15 -&gt; 11 -&gt; 10 -&gt; 7 -&gt; 4 -&gt; 1 -&gt; 2 -&gt; 5 -&gt; 6</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>0.04253435134887695</v>
+      <c r="B8" t="n">
+        <v>2599.766666666667</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2811</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2395</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.04398438930511474</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2434.8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2550</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2294</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.04370657602945963</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2456.833333333333</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2761</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2082</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.04420396486918132</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2268.2</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2326</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2230</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.0409963607788086</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajustes nos algoritmos BFS e DFS  alem de criar um novo conjunto de testes unitarios para a tabela de resultados!
</commit_message>
<xml_diff>
--- a/Algoritmo_Rota/Planilhas/A_Estrela_Euclidiano/PLN_42_10.xlsx
+++ b/Algoritmo_Rota/Planilhas/A_Estrela_Euclidiano/PLN_42_10.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,25 +424,20 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Índice</t>
+          <t>Qtd_Nós</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
+        <is>
+          <t>Ativos</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>Distancia</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>max</t>
-        </is>
-      </c>
       <c r="D1" t="inlineStr">
-        <is>
-          <t>min</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
         <is>
           <t>Tempo</t>
         </is>
@@ -450,172 +445,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B2" t="n">
-        <v>2422.766666666667</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>2679</v>
+        <v>3144</v>
       </c>
       <c r="D2" t="n">
-        <v>2268</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.02985102335611979</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2425</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2552</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2364</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.0295865535736084</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>2287.866666666667</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2411</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2171</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.0326434055964152</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>2155.466666666667</v>
-      </c>
-      <c r="C5" t="n">
-        <v>2234</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2080</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.02993044058481852</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>2157.3</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2251</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1922</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.03292287190755208</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1786.433333333333</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1949</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1614</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.0391965389251709</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>2599.766666666667</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2811</v>
-      </c>
-      <c r="D8" t="n">
-        <v>2395</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.04398438930511474</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>2434.8</v>
-      </c>
-      <c r="C9" t="n">
-        <v>2550</v>
-      </c>
-      <c r="D9" t="n">
-        <v>2294</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.04370657602945963</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>2456.833333333333</v>
-      </c>
-      <c r="C10" t="n">
-        <v>2761</v>
-      </c>
-      <c r="D10" t="n">
-        <v>2082</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.04420396486918132</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>2268.2</v>
-      </c>
-      <c r="C11" t="n">
-        <v>2326</v>
-      </c>
-      <c r="D11" t="n">
-        <v>2230</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.0409963607788086</v>
+        <v>0.02959275245666504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>